<commit_message>
add title to all links
</commit_message>
<xml_diff>
--- a/Modèle+analyse+SEO+et+accessibilité+(1).xlsx
+++ b/Modèle+analyse+SEO+et+accessibilité+(1).xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\houri\OneDrive\Desktop\openclassroom\Starting website\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\houri\OneDrive\Desktop\openclassroom\abdelhakhamdouni_4_03082020\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7837D9FC-1F5A-42A9-A1DA-7E82C6210712}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3174F204-0FD1-40B5-B05E-49DCB69F4A3E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -533,13 +532,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="27" style="3" customWidth="1"/>
+    <col min="1" max="1" width="21.77734375" style="3" customWidth="1"/>
     <col min="2" max="2" width="21.6640625" style="3" customWidth="1"/>
     <col min="3" max="3" width="31.44140625" style="3" customWidth="1"/>
     <col min="4" max="4" width="43.33203125" style="3" customWidth="1"/>

</xml_diff>